<commit_message>
updates trial 19 with weights from run on lab computer
</commit_message>
<xml_diff>
--- a/data/Fall2024/Network Motif Comparison - 3 gene, 4 node networks/Analysis/Original-Runs_P-constant_summary.xlsx
+++ b/data/Fall2024/Network Motif Comparison - 3 gene, 4 node networks/Analysis/Original-Runs_P-constant_summary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kdahlqui\Documents\Travel-Conferences\BOSC_ISMB_2025\21 original runs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nikki\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A9F715F-658D-4277-AE02-016AE1B0354C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC678672-A650-4B38-8AF1-D09589CFEF4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" tabRatio="845" xr2:uid="{61DF7949-D53D-4105-9735-EE06691314FF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="845" activeTab="19" xr2:uid="{61DF7949-D53D-4105-9735-EE06691314FF}"/>
   </bookViews>
   <sheets>
     <sheet name="P Constant" sheetId="1" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="10">
   <si>
     <t>Trial</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t>reran data because no data in folder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">updated with output from lab computer </t>
   </si>
 </sst>
 </file>
@@ -157,12 +160,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -401,7 +405,7 @@
                   <c:v>3.6303566876897907E-6</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>7.3397955041235052E-6</c:v>
+                  <c:v>2.5315618223864992E-5</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>5.3388772082334952E-3</c:v>
@@ -566,6 +570,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -573,7 +578,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1511,17 +1515,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7478D67-BA7D-48FA-92AF-8000621A116E}">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D24" sqref="D24:E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1535,7 +1539,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>16</v>
       </c>
@@ -1550,7 +1554,7 @@
         <v>9.9181798458956543</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>15</v>
       </c>
@@ -1565,7 +1569,7 @@
         <v>4.3002266476297253</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>7</v>
       </c>
@@ -1580,7 +1584,7 @@
         <v>3.4340534828846362E-8</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>8</v>
       </c>
@@ -1595,7 +1599,7 @@
         <v>3.0404652118011022E-6</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>13</v>
       </c>
@@ -1610,7 +1614,7 @@
         <v>3.6303566876897907E-6</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>12</v>
       </c>
@@ -1625,7 +1629,7 @@
         <v>2.8490723934436047E-7</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>20</v>
       </c>
@@ -1640,7 +1644,7 @@
         <v>4.5123729600762591E-10</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>9</v>
       </c>
@@ -1655,7 +1659,7 @@
         <v>8.1226108532573268E-10</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>3</v>
       </c>
@@ -1670,7 +1674,7 @@
         <v>9.2077725948340428E-9</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1685,7 +1689,7 @@
         <v>3.6031259077816692E-8</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>6</v>
       </c>
@@ -1700,7 +1704,7 @@
         <v>5.3388772082334952E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>4</v>
       </c>
@@ -1715,7 +1719,7 @@
         <v>1.1991863700778435E-9</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>5</v>
       </c>
@@ -1730,13 +1734,13 @@
         <v>1.0115308916029265E-9</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>19</v>
       </c>
       <c r="B15" s="1">
         <f>'19'!B16</f>
-        <v>7.3397955041235052E-6</v>
+        <v>2.5315618223864992E-5</v>
       </c>
       <c r="D15">
         <v>14</v>
@@ -1745,7 +1749,7 @@
         <v>4.4998625069898432</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>11</v>
       </c>
@@ -1760,7 +1764,7 @@
         <v>8.6778700869389412E-11</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>21</v>
       </c>
@@ -1775,7 +1779,7 @@
         <v>4.6698300773274395E-11</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>2</v>
       </c>
@@ -1790,7 +1794,7 @@
         <v>4.5015572260013741</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>14</v>
       </c>
@@ -1805,7 +1809,7 @@
         <v>7.1053368112401367</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>17</v>
       </c>
@@ -1820,7 +1824,7 @@
         <v>7.3397955041235052E-6</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>18</v>
       </c>
@@ -1835,7 +1839,7 @@
         <v>1.7491420541030022E-9</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>1</v>
       </c>
@@ -1850,7 +1854,7 @@
         <v>1.1925822189679345</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D23" t="s">
         <v>2</v>
       </c>
@@ -1859,7 +1863,7 @@
         <v>1.5010999292568545</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D24" t="s">
         <v>3</v>
       </c>
@@ -1885,9 +1889,9 @@
       <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -1901,7 +1905,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1915,7 +1919,7 @@
         <v>0.99997339743445735</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1929,7 +1933,7 @@
         <v>1.9999722285275572</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1943,7 +1947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -1957,7 +1961,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -1971,7 +1975,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -1985,7 +1989,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -1999,7 +2003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B12">
         <f>(B8-B2)^2</f>
         <v>0</v>
@@ -2013,7 +2017,7 @@
         <v>7.0769649345125211E-10</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B13">
         <f t="shared" ref="B13:D14" si="1">(B9-B3)^2</f>
         <v>0</v>
@@ -2027,7 +2031,7 @@
         <v>7.7125468164213618E-10</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B14">
         <f>(B10-B4)^2</f>
         <v>0</v>
@@ -2041,7 +2045,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B16" s="2">
         <f>SUM(B12:D14)</f>
         <v>9.2077725948340428E-9</v>
@@ -2060,9 +2064,9 @@
       <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -2076,7 +2080,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2090,7 +2094,7 @@
         <v>1.0001088325237473</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -2104,7 +2108,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -2118,7 +2122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -2132,7 +2136,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -2146,7 +2150,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -2160,7 +2164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -2174,7 +2178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B12">
         <f>(B8-B2)^2</f>
         <v>0</v>
@@ -2188,7 +2192,7 @@
         <v>1.184451822520029E-8</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B13">
         <f t="shared" ref="B13:D14" si="1">(B9-B3)^2</f>
         <v>1.6276466472168673E-9</v>
@@ -2202,7 +2206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B14">
         <f>(B10-B4)^2</f>
         <v>1.1977806650647838E-8</v>
@@ -2216,7 +2220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B16" s="2">
         <f>SUM(B12:D14)</f>
         <v>3.6031259077816692E-8</v>
@@ -2235,9 +2239,9 @@
       <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -2251,7 +2255,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2265,7 +2269,7 @@
         <v>-0.9943763078157084</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -2279,7 +2283,7 @@
         <v>1.9668949584557416</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -2293,7 +2297,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -2307,7 +2311,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -2321,7 +2325,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -2335,7 +2339,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -2349,7 +2353,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B12">
         <f>(B8-B2)^2</f>
         <v>4.0403064342122872E-3</v>
@@ -2363,7 +2367,7 @@
         <v>3.1625913783662374E-5</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B13">
         <f t="shared" ref="B13:D14" si="1">(B9-B3)^2</f>
         <v>0</v>
@@ -2377,7 +2381,7 @@
         <v>1.0959437756470757E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B14">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2391,7 +2395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B16" s="2">
         <f>SUM(B12:D14)</f>
         <v>5.3388772082334952E-3</v>
@@ -2410,9 +2414,9 @@
       <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -2426,7 +2430,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2440,7 +2444,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -2454,7 +2458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -2468,7 +2472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -2482,7 +2486,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -2496,7 +2500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -2510,7 +2514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -2524,7 +2528,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B12">
         <f>(B8-B2)^2</f>
         <v>0</v>
@@ -2538,7 +2542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B13">
         <f t="shared" ref="B13:D14" si="1">(B9-B3)^2</f>
         <v>4.3684472315875073E-10</v>
@@ -2552,7 +2556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B14">
         <f t="shared" si="1"/>
         <v>5.6744068923237394E-10</v>
@@ -2566,7 +2570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B16" s="2">
         <f>SUM(B12:D14)</f>
         <v>1.1991863700778435E-9</v>
@@ -2585,9 +2589,9 @@
       <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -2601,7 +2605,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2615,7 +2619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -2629,7 +2633,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -2643,7 +2647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -2657,7 +2661,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -2671,7 +2675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -2685,7 +2689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -2699,7 +2703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B12">
         <f>(B8-B2)^2</f>
         <v>1.0421294738641679E-10</v>
@@ -2713,7 +2717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B13">
         <f t="shared" ref="B13:D14" si="1">(B9-B3)^2</f>
         <v>0</v>
@@ -2727,7 +2731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B14">
         <f t="shared" si="1"/>
         <v>7.1450130285085365E-10</v>
@@ -2741,7 +2745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B16" s="2">
         <f>SUM(B12:D14)</f>
         <v>1.0115308916029265E-9</v>
@@ -2760,9 +2764,9 @@
       <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -2776,7 +2780,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2790,7 +2794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -2804,7 +2808,7 @@
         <v>1.9993134279659068</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -2818,7 +2822,7 @@
         <v>-0.49991474948644876</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -2832,7 +2836,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -2846,7 +2850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -2860,7 +2864,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -2874,7 +2878,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B12">
         <f>(B8-B2)^2</f>
         <v>8.2923690721480968E-9</v>
@@ -2888,7 +2892,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B13">
         <f t="shared" ref="B13:D14" si="1">(B9-B3)^2</f>
         <v>0</v>
@@ -2902,7 +2906,7 @@
         <v>4.7138115799883178E-7</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B14">
         <f t="shared" si="1"/>
         <v>2.2501177715893195</v>
@@ -2916,7 +2920,7 @@
         <v>2.2497442557269967</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B16" s="2">
         <f>SUM(B12:D14)</f>
         <v>4.4998625069898432</v>
@@ -2935,9 +2939,9 @@
       <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -2951,7 +2955,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2965,7 +2969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -2979,7 +2983,7 @@
         <v>1.9999940368885727</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -2993,7 +2997,7 @@
         <v>0.99999430923095767</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -3007,7 +3011,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -3021,7 +3025,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -3035,7 +3039,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -3049,7 +3053,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B12">
         <f>(B8-B2)^2</f>
         <v>0</v>
@@ -3063,7 +3067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B13">
         <f t="shared" ref="B13:D14" si="1">(B9-B3)^2</f>
         <v>0</v>
@@ -3077,7 +3081,7 @@
         <v>3.5558697894509646E-11</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B14">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3091,7 +3095,7 @@
         <v>3.2384852293169448E-11</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B16" s="2">
         <f>SUM(B12:D14)</f>
         <v>8.6778700869389412E-11</v>
@@ -3110,9 +3114,9 @@
       <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -3126,7 +3130,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -3140,7 +3144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -3154,7 +3158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -3168,7 +3172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -3182,7 +3186,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -3196,7 +3200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -3210,7 +3214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -3224,7 +3228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B12">
         <f>(B8-B2)^2</f>
         <v>0</v>
@@ -3238,7 +3242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B13">
         <f t="shared" ref="B13:D14" si="1">(B9-B3)^2</f>
         <v>0</v>
@@ -3252,7 +3256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B14">
         <f t="shared" si="1"/>
         <v>2.2403791125511522E-11</v>
@@ -3266,7 +3270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B16" s="2">
         <f>SUM(B12:D14)</f>
         <v>4.6698300773274395E-11</v>
@@ -3285,9 +3289,9 @@
       <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -3301,7 +3305,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -3315,7 +3319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -3329,7 +3333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -3343,7 +3347,7 @@
         <v>-0.50022622031849817</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -3357,7 +3361,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -3371,7 +3375,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -3385,7 +3389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -3399,7 +3403,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B12">
         <f>(B8-B2)^2</f>
         <v>3.7694235587884804E-8</v>
@@ -3413,7 +3417,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B13">
         <f t="shared" ref="B13:D14" si="1">(B9-B3)^2</f>
         <v>5.2899527938223088E-7</v>
@@ -3427,7 +3431,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B14">
         <f t="shared" si="1"/>
         <v>2.2508779471807325</v>
@@ -3441,7 +3445,7 @@
         <v>2.2506787121311271</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B16" s="2">
         <f>SUM(B12:D14)</f>
         <v>4.5015572260013741</v>
@@ -3460,9 +3464,9 @@
       <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -3476,7 +3480,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -3490,7 +3494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -3504,7 +3508,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -3518,7 +3522,7 @@
         <v>-0.18842641396375912</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -3532,7 +3536,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -3546,7 +3550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -3560,7 +3564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -3574,7 +3578,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B12">
         <f>(B8-B2)^2</f>
         <v>0</v>
@@ -3588,7 +3592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B13">
         <f t="shared" ref="B13:D14" si="1">(B9-B3)^2</f>
         <v>0</v>
@@ -3602,7 +3606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B14">
         <f t="shared" si="1"/>
         <v>4.2805572777593568</v>
@@ -3616,13 +3620,13 @@
         <v>1.4123573414067601</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B16" s="2">
         <f>SUM(B12:D14)</f>
         <v>7.1053368112401367</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" s="4"/>
     </row>
   </sheetData>
@@ -3638,9 +3642,9 @@
       <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -3654,7 +3658,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -3668,7 +3672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -3682,7 +3686,7 @@
         <v>2.4270519913476594E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -3696,7 +3700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -3710,7 +3714,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -3724,7 +3728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -3738,7 +3742,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -3752,7 +3756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B12">
         <f>(B8-B2)^2</f>
         <v>0</v>
@@ -3766,7 +3770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B13">
         <f t="shared" ref="B13:D14" si="1">(B9-B3)^2</f>
         <v>0.94694657218292799</v>
@@ -3780,7 +3784,7 @@
         <v>0.95204801830991725</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B14">
         <f>(B10-B4)^2</f>
         <v>4.0061068681478744</v>
@@ -3794,7 +3798,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B16" s="2">
         <f>SUM(B12:D14)</f>
         <v>9.9181798458956543</v>
@@ -3807,71 +3811,74 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A76EDBDA-A255-485C-A114-9E4EBC1235F8}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2">
-        <v>-0.9979922891579287</v>
-      </c>
-      <c r="C2">
-        <v>-1.9982874245768647</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>1.9993898451341277</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>1.0000607382785245</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="5">
+        <v>-0.99632519127464669</v>
+      </c>
+      <c r="C2" s="5">
+        <v>-1.9965786036919344</v>
+      </c>
+      <c r="D2" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="5">
+        <v>0</v>
+      </c>
+      <c r="C3" s="5">
+        <v>0</v>
+      </c>
+      <c r="D3" s="5">
+        <v>2.0003228159575697</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="5">
+        <v>0</v>
+      </c>
+      <c r="C4" s="5">
+        <v>0</v>
+      </c>
+      <c r="D4" s="5">
+        <v>1.0000351598723789</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -3885,7 +3892,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -3899,7 +3906,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -3913,7 +3920,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -3927,21 +3934,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B12">
         <f>(B8-B2)^2</f>
-        <v>4.0309028253706381E-6</v>
+        <v>1.3504219167932795E-5</v>
       </c>
       <c r="C12">
         <f t="shared" ref="C12:D12" si="0">(C8-C2)^2</f>
-        <v>2.932914579927047E-6</v>
+        <v>1.1705952696844878E-5</v>
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B13">
         <f t="shared" ref="B13:D14" si="1">(B9-B3)^2</f>
         <v>0</v>
@@ -3952,10 +3959,10 @@
       </c>
       <c r="D13">
         <f t="shared" si="1"/>
-        <v>3.7228896034770257E-7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1.0421014246162073E-7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B14">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3966,21 +3973,29 @@
       </c>
       <c r="D14">
         <f t="shared" si="1"/>
-        <v>3.6891384781180224E-9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1.2362166257004066E-9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B16" s="2">
         <f>SUM(B12:D14)</f>
-        <v>7.3397955041235052E-6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2.5315618223864992E-5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
         <v>45847</v>
       </c>
       <c r="B17" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="4">
+        <v>45923</v>
+      </c>
+      <c r="B18" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -3996,9 +4011,9 @@
       <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -4012,7 +4027,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -4026,7 +4041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -4040,7 +4055,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -4054,7 +4069,7 @@
         <v>1.0000175564579665</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -4068,7 +4083,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -4082,7 +4097,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -4096,7 +4111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -4110,7 +4125,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B12">
         <f>(B8-B2)^2</f>
         <v>0</v>
@@ -4124,7 +4139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B13">
         <f t="shared" ref="B13:D14" si="1">(B9-B3)^2</f>
         <v>9.4224826747076011E-10</v>
@@ -4138,7 +4153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B14">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4152,7 +4167,7 @@
         <v>3.0822921633045451E-10</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B16" s="2">
         <f>SUM(B12:D14)</f>
         <v>1.7491420541030022E-9</v>
@@ -4171,9 +4186,9 @@
       <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -4187,7 +4202,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -4201,7 +4216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -4215,7 +4230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -4229,7 +4244,7 @@
         <v>0.9999258192369036</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -4243,7 +4258,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -4257,7 +4272,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -4271,7 +4286,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -4285,7 +4300,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B12">
         <f>(B8-B2)^2</f>
         <v>0</v>
@@ -4299,7 +4314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B13">
         <f t="shared" ref="B13:D14" si="1">(B9-B3)^2</f>
         <v>0.11993824765256311</v>
@@ -4313,7 +4328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B14">
         <f t="shared" si="1"/>
         <v>1.0726439655822539</v>
@@ -4327,7 +4342,7 @@
         <v>5.50278561356402E-9</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B16" s="2">
         <f>SUM(B12:D14)</f>
         <v>1.1925822189679345</v>
@@ -4346,9 +4361,9 @@
       <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -4362,7 +4377,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -4376,7 +4391,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -4390,7 +4405,7 @@
         <v>0.22305858959594416</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -4404,7 +4419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -4418,7 +4433,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -4432,7 +4447,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -4446,7 +4461,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -4460,7 +4475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B12">
         <f>(B8-B2)^2</f>
         <v>0</v>
@@ -4474,7 +4489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B13">
         <f t="shared" ref="B13:D14" si="1">(B9-B3)^2</f>
         <v>3.0934121484944019</v>
@@ -4488,7 +4503,7 @@
         <v>0.60363795520064356</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B14">
         <f>(B10-B4)^2</f>
         <v>0</v>
@@ -4502,7 +4517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B16" s="2">
         <f>SUM(B12:D14)</f>
         <v>4.3002266476297253</v>
@@ -4521,9 +4536,9 @@
       <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -4537,7 +4552,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -4551,7 +4566,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -4565,7 +4580,7 @@
         <v>1.0000339656771842</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -4579,7 +4594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -4593,7 +4608,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -4607,7 +4622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -4621,7 +4636,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -4635,7 +4650,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B12">
         <f>(B8-B2)^2</f>
         <v>1.0792552964615165E-8</v>
@@ -4649,7 +4664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B13">
         <f t="shared" ref="B13:D14" si="1">(B9-B3)^2</f>
         <v>0</v>
@@ -4663,7 +4678,7 @@
         <v>1.1536672265790267E-9</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B14">
         <f>(B10-B4)^2</f>
         <v>5.0911418357998612E-9</v>
@@ -4677,7 +4692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B16" s="2">
         <f>SUM(B12:D14)</f>
         <v>3.4340534828846362E-8</v>
@@ -4696,9 +4711,9 @@
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -4712,7 +4727,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -4726,7 +4741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -4740,7 +4755,7 @@
         <v>0.99928392523804233</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -4754,7 +4769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -4768,7 +4783,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -4782,7 +4797,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -4796,7 +4811,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -4810,7 +4825,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B12">
         <f>(B8-B2)^2</f>
         <v>0</v>
@@ -4824,7 +4839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B13">
         <f t="shared" ref="B13:D14" si="1">(B9-B3)^2</f>
         <v>0</v>
@@ -4838,7 +4853,7 @@
         <v>5.1276306471274036E-7</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B14">
         <f>(B10-B4)^2</f>
         <v>0</v>
@@ -4852,7 +4867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B16" s="2">
         <f>SUM(B12:D14)</f>
         <v>3.0404652118011022E-6</v>
@@ -4869,9 +4884,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -4885,7 +4900,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -4899,7 +4914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -4913,7 +4928,7 @@
         <v>1.0001252062292589</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -4927,7 +4942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -4941,7 +4956,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -4955,7 +4970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -4969,7 +4984,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -4983,7 +4998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B12">
         <f>(B8-B2)^2</f>
         <v>2.257133838201372E-6</v>
@@ -4997,7 +5012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B13">
         <f t="shared" ref="B13:D14" si="1">(B9-B3)^2</f>
         <v>0</v>
@@ -5011,7 +5026,7 @@
         <v>1.5676599845240738E-8</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B14">
         <f>(B10-B4)^2</f>
         <v>0</v>
@@ -5025,7 +5040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B16" s="2">
         <f>SUM(B12:D14)</f>
         <v>3.6303566876897907E-6</v>
@@ -5044,9 +5059,9 @@
       <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -5060,7 +5075,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -5074,7 +5089,7 @@
         <v>-0.99977725205514922</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -5088,7 +5103,7 @@
         <v>1.9996612130484597</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -5102,7 +5117,7 @@
         <v>-1.9996733189877614</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -5116,7 +5131,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -5130,7 +5145,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -5144,7 +5159,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -5158,7 +5173,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B12">
         <f>(B8-B2)^2</f>
         <v>0</v>
@@ -5172,7 +5187,7 @@
         <v>4.9616646935244487E-8</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B13">
         <f t="shared" ref="B13:D14" si="1">(B9-B3)^2</f>
         <v>0</v>
@@ -5186,7 +5201,7 @@
         <v>1.1477659853398743E-7</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B14">
         <f>(B10-B4)^2</f>
         <v>0</v>
@@ -5200,7 +5215,7 @@
         <v>1.0672048375726891E-7</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B16" s="2">
         <f>SUM(B12:D14)</f>
         <v>2.8490723934436047E-7</v>
@@ -5219,9 +5234,9 @@
       <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -5235,7 +5250,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -5249,7 +5264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -5263,7 +5278,7 @@
         <v>0.99999677456410552</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -5277,7 +5292,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -5291,7 +5306,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -5305,7 +5320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -5319,7 +5334,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -5333,7 +5348,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B12">
         <f>(B8-B2)^2</f>
         <v>9.0355165274668185E-11</v>
@@ -5347,7 +5362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B13">
         <f t="shared" ref="B13:D14" si="1">(B9-B3)^2</f>
         <v>2.5667573193892489E-10</v>
@@ -5361,7 +5376,7 @@
         <v>1.040343670941783E-11</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B14">
         <f>(B10-B4)^2</f>
         <v>0</v>
@@ -5375,7 +5390,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B16" s="2">
         <f>SUM(B12:D14)</f>
         <v>4.5123729600762591E-10</v>
@@ -5394,9 +5409,9 @@
       <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -5410,7 +5425,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -5424,7 +5439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -5438,7 +5453,7 @@
         <v>0.99999805152576005</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -5452,7 +5467,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -5466,7 +5481,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -5480,7 +5495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -5494,7 +5509,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -5508,7 +5523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B12">
         <f>(B8-B2)^2</f>
         <v>0</v>
@@ -5522,7 +5537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B13">
         <f t="shared" ref="B13:D14" si="1">(B9-B3)^2</f>
         <v>0</v>
@@ -5536,7 +5551,7 @@
         <v>3.7965518637661828E-12</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B14">
         <f>(B10-B4)^2</f>
         <v>2.4737206257391508E-10</v>
@@ -5550,7 +5565,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B16" s="2">
         <f>SUM(B12:D14)</f>
         <v>8.1226108532573268E-10</v>
@@ -5562,6 +5577,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="070f1269-45c1-4463-99ba-5dc4e57c7dff" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008DB5B7ED115EF04980BBFAFC51672553" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="43a679fe5cbd3b1dc01cea5b3bb6a16a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="070f1269-45c1-4463-99ba-5dc4e57c7dff" xmlns:ns4="7bf50b4b-6300-445a-aea1-306a2291592c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b0963d0390b393dc53bf13ff5a8315f4" ns3:_="" ns4:_="">
     <xsd:import namespace="070f1269-45c1-4463-99ba-5dc4e57c7dff"/>
@@ -5756,24 +5788,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="070f1269-45c1-4463-99ba-5dc4e57c7dff" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2EE723E-1688-4D1F-8FE6-FDF46584855C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FAD4690-B959-480E-AC59-DDDE87F8E768}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="070f1269-45c1-4463-99ba-5dc4e57c7dff"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{02EB7017-44D4-47C1-BB45-296DD07AFBB9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5790,22 +5823,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FAD4690-B959-480E-AC59-DDDE87F8E768}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="070f1269-45c1-4463-99ba-5dc4e57c7dff"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2EE723E-1688-4D1F-8FE6-FDF46584855C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Edited bar graph to be sorted correctly and include all trials
</commit_message>
<xml_diff>
--- a/data/Fall2024/Network Motif Comparison - 3 gene, 4 node networks/Analysis/Original-Runs_P-constant_summary.xlsx
+++ b/data/Fall2024/Network Motif Comparison - 3 gene, 4 node networks/Analysis/Original-Runs_P-constant_summary.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29127"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nikki\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BDD668A-1F8E-4AEA-B7FE-8ABA836A06CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" tabRatio="845" xr2:uid="{61DF7949-D53D-4105-9735-EE06691314FF}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="11715" windowHeight="12330" tabRatio="845"/>
   </bookViews>
   <sheets>
     <sheet name="P Constant" sheetId="1" r:id="rId1"/>
@@ -93,11 +87,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.00000E+00"/>
+    <numFmt numFmtId="164" formatCode="0.00000E+00"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -171,17 +165,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="3" xr:uid="{70519227-5B63-4686-ADE9-D4CF5CB72DF2}"/>
-    <cellStyle name="Normal 3" xfId="2" xr:uid="{6D324F20-C91C-4E45-A4F0-8B5D47920066}"/>
-    <cellStyle name="Normal 3 2" xfId="4" xr:uid="{7363577E-F7A0-4CDB-B7F4-B9089FCE3807}"/>
-    <cellStyle name="Normal 4" xfId="1" xr:uid="{530E491E-9E52-4105-A481-D94D8643FA3F}"/>
+    <cellStyle name="Normal 2" xfId="3"/>
+    <cellStyle name="Normal 3" xfId="2"/>
+    <cellStyle name="Normal 3 2" xfId="4"/>
+    <cellStyle name="Normal 4" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -197,7 +191,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -236,6 +230,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -244,26 +239,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -298,10 +273,10 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>'P Constant'!$A$2:$A$22</c:f>
+              <c:f>'P Constant'!$A$2:$A$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="22"/>
                 <c:pt idx="0">
                   <c:v>16</c:v>
                 </c:pt>
@@ -365,15 +340,18 @@
                 <c:pt idx="20">
                   <c:v>18</c:v>
                 </c:pt>
+                <c:pt idx="21">
+                  <c:v>1</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'P Constant'!$B$2:$B$22</c:f>
+              <c:f>'P Constant'!$B$2:$B$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="22"/>
                 <c:pt idx="0">
                   <c:v>4.6698300773274395E-11</c:v>
                 </c:pt>
@@ -437,10 +415,13 @@
                 <c:pt idx="20">
                   <c:v>7.1053368112401367</c:v>
                 </c:pt>
+                <c:pt idx="21">
+                  <c:v>9.9181798458956543</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-3AE6-4C22-9488-42930035D488}"/>
             </c:ext>
@@ -456,11 +437,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1279891743"/>
-        <c:axId val="1279897503"/>
+        <c:axId val="81480192"/>
+        <c:axId val="83817536"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1279891743"/>
+        <c:axId val="81480192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -503,7 +484,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1279897503"/>
+        <c:crossAx val="83817536"/>
         <c:crossesAt val="1.0000000000000007E-13"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -511,7 +492,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1279897503"/>
+        <c:axId val="83817536"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -565,7 +546,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1279891743"/>
+        <c:crossAx val="81480192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -580,7 +561,7 @@
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
-    <c:extLst>
+    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
@@ -1184,7 +1165,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6F86DA50-4012-DB17-F88E-613B20E279DF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6F86DA50-4012-DB17-F88E-613B20E279DF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1514,27 +1495,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7478D67-BA7D-48FA-92AF-8000621A116E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="7.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.5" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="2" customFormat="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1548,7 +1529,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5">
       <c r="A2" s="1">
         <v>16</v>
       </c>
@@ -1563,7 +1544,7 @@
         <v>9.9181798458956543</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5">
       <c r="A3" s="1">
         <v>15</v>
       </c>
@@ -1578,7 +1559,7 @@
         <v>4.3002266476297253</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5">
       <c r="A4" s="1">
         <v>7</v>
       </c>
@@ -1593,7 +1574,7 @@
         <v>3.4340534828846362E-8</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5">
       <c r="A5" s="1">
         <v>8</v>
       </c>
@@ -1608,7 +1589,7 @@
         <v>3.0404652118011022E-6</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5">
       <c r="A6" s="1">
         <v>13</v>
       </c>
@@ -1623,7 +1604,7 @@
         <v>3.6303566876897907E-6</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5">
       <c r="A7" s="1">
         <v>12</v>
       </c>
@@ -1638,7 +1619,7 @@
         <v>2.8490723934436047E-7</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5">
       <c r="A8" s="1">
         <v>20</v>
       </c>
@@ -1653,7 +1634,7 @@
         <v>4.5123729600762591E-10</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5">
       <c r="A9" s="1">
         <v>22</v>
       </c>
@@ -1668,7 +1649,7 @@
         <v>8.1226108532573268E-10</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1683,7 +1664,7 @@
         <v>9.2077725948340428E-9</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5">
       <c r="A11" s="1">
         <v>3</v>
       </c>
@@ -1698,7 +1679,7 @@
         <v>3.6031259077816692E-8</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1713,7 +1694,7 @@
         <v>5.3388772082334952E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5">
       <c r="A13" s="1">
         <v>6</v>
       </c>
@@ -1728,7 +1709,7 @@
         <v>1.1991863700778435E-9</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5">
       <c r="A14" s="1">
         <v>4</v>
       </c>
@@ -1743,7 +1724,7 @@
         <v>1.0115308916029265E-9</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5">
       <c r="A15" s="1">
         <v>5</v>
       </c>
@@ -1758,7 +1739,7 @@
         <v>4.4998625069898432</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5">
       <c r="A16" s="1">
         <v>19</v>
       </c>
@@ -1773,7 +1754,7 @@
         <v>8.6778700869389412E-11</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5">
       <c r="A17" s="1">
         <v>11</v>
       </c>
@@ -1788,7 +1769,7 @@
         <v>4.6698300773274395E-11</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5">
       <c r="A18" s="1">
         <v>21</v>
       </c>
@@ -1803,7 +1784,7 @@
         <v>4.5015572260013741</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5">
       <c r="A19" s="1">
         <v>2</v>
       </c>
@@ -1818,7 +1799,7 @@
         <v>7.1053368112401367</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5">
       <c r="A20" s="1">
         <v>14</v>
       </c>
@@ -1833,7 +1814,7 @@
         <v>7.3397955041235052E-6</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5">
       <c r="A21" s="1">
         <v>17</v>
       </c>
@@ -1848,7 +1829,7 @@
         <v>1.7491420541030022E-9</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5">
       <c r="A22" s="1">
         <v>18</v>
       </c>
@@ -1863,7 +1844,7 @@
         <v>1.1925822189679345</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5">
       <c r="A23" s="1">
         <v>1</v>
       </c>
@@ -1878,7 +1859,7 @@
         <v>2.5939981710941708E-9</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5">
       <c r="D24" t="s">
         <v>2</v>
       </c>
@@ -1887,7 +1868,7 @@
         <v>1.4328681144085429</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5">
       <c r="D25" t="s">
         <v>3</v>
       </c>
@@ -1897,7 +1878,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B23">
+  <sortState ref="A2:B23">
     <sortCondition ref="B2:B23"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1906,16 +1887,16 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83615C64-E794-4FBF-9071-AD2A44D1D0A5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -1929,7 +1910,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1943,7 +1924,7 @@
         <v>0.99997339743445735</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1957,7 +1938,7 @@
         <v>1.9999722285275572</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1971,7 +1952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -1985,7 +1966,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -1999,7 +1980,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -2013,7 +1994,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -2027,7 +2008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4">
       <c r="B12">
         <f>(B8-B2)^2</f>
         <v>0</v>
@@ -2041,7 +2022,7 @@
         <v>7.0769649345125211E-10</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4">
       <c r="B13">
         <f t="shared" ref="B13:D14" si="1">(B9-B3)^2</f>
         <v>0</v>
@@ -2055,7 +2036,7 @@
         <v>7.7125468164213618E-10</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4">
       <c r="B14">
         <f>(B10-B4)^2</f>
         <v>0</v>
@@ -2069,7 +2050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4">
       <c r="B16" s="2">
         <f>SUM(B12:D14)</f>
         <v>9.2077725948340428E-9</v>
@@ -2081,16 +2062,16 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40157B9F-6434-4685-B5EC-1BE86917077B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -2104,7 +2085,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2118,7 +2099,7 @@
         <v>1.0001088325237473</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -2132,7 +2113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -2146,7 +2127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -2160,7 +2141,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -2174,7 +2155,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -2188,7 +2169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -2202,7 +2183,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4">
       <c r="B12">
         <f>(B8-B2)^2</f>
         <v>0</v>
@@ -2216,7 +2197,7 @@
         <v>1.184451822520029E-8</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4">
       <c r="B13">
         <f t="shared" ref="B13:D14" si="1">(B9-B3)^2</f>
         <v>1.6276466472168673E-9</v>
@@ -2230,7 +2211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4">
       <c r="B14">
         <f>(B10-B4)^2</f>
         <v>1.1977806650647838E-8</v>
@@ -2244,7 +2225,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4">
       <c r="B16" s="2">
         <f>SUM(B12:D14)</f>
         <v>3.6031259077816692E-8</v>
@@ -2256,16 +2237,16 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA995C32-351D-49BE-93C9-576C97468297}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -2279,7 +2260,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2293,7 +2274,7 @@
         <v>-0.9943763078157084</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -2307,7 +2288,7 @@
         <v>1.9668949584557416</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -2321,7 +2302,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -2335,7 +2316,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -2349,7 +2330,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -2363,7 +2344,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -2377,7 +2358,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4">
       <c r="B12">
         <f>(B8-B2)^2</f>
         <v>4.0403064342122872E-3</v>
@@ -2391,7 +2372,7 @@
         <v>3.1625913783662374E-5</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4">
       <c r="B13">
         <f t="shared" ref="B13:D14" si="1">(B9-B3)^2</f>
         <v>0</v>
@@ -2405,7 +2386,7 @@
         <v>1.0959437756470757E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4">
       <c r="B14">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2419,7 +2400,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4">
       <c r="B16" s="2">
         <f>SUM(B12:D14)</f>
         <v>5.3388772082334952E-3</v>
@@ -2431,16 +2412,16 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12EF0B3D-B400-4975-8CA7-B989EBF30B53}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -2454,7 +2435,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2468,7 +2449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -2482,7 +2463,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -2496,7 +2477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -2510,7 +2491,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -2524,7 +2505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -2538,7 +2519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -2552,7 +2533,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4">
       <c r="B12">
         <f>(B8-B2)^2</f>
         <v>0</v>
@@ -2566,7 +2547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4">
       <c r="B13">
         <f t="shared" ref="B13:D14" si="1">(B9-B3)^2</f>
         <v>4.3684472315875073E-10</v>
@@ -2580,7 +2561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4">
       <c r="B14">
         <f t="shared" si="1"/>
         <v>5.6744068923237394E-10</v>
@@ -2594,7 +2575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4">
       <c r="B16" s="2">
         <f>SUM(B12:D14)</f>
         <v>1.1991863700778435E-9</v>
@@ -2606,16 +2587,16 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE8DD21A-91B9-413D-87A7-237727AE6C19}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -2629,7 +2610,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2643,7 +2624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -2657,7 +2638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -2671,7 +2652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -2685,7 +2666,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -2699,7 +2680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -2713,7 +2694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -2727,7 +2708,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4">
       <c r="B12">
         <f>(B8-B2)^2</f>
         <v>1.0421294738641679E-10</v>
@@ -2741,7 +2722,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4">
       <c r="B13">
         <f t="shared" ref="B13:D14" si="1">(B9-B3)^2</f>
         <v>0</v>
@@ -2755,7 +2736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4">
       <c r="B14">
         <f t="shared" si="1"/>
         <v>7.1450130285085365E-10</v>
@@ -2769,7 +2750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4">
       <c r="B16" s="2">
         <f>SUM(B12:D14)</f>
         <v>1.0115308916029265E-9</v>
@@ -2781,16 +2762,16 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{142147BB-8850-42AC-BF7C-800B472E78BD}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -2804,7 +2785,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2818,7 +2799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -2832,7 +2813,7 @@
         <v>1.9993134279659068</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -2846,7 +2827,7 @@
         <v>-0.49991474948644876</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -2860,7 +2841,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -2874,7 +2855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -2888,7 +2869,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -2902,7 +2883,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4">
       <c r="B12">
         <f>(B8-B2)^2</f>
         <v>8.2923690721480968E-9</v>
@@ -2916,7 +2897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4">
       <c r="B13">
         <f t="shared" ref="B13:D14" si="1">(B9-B3)^2</f>
         <v>0</v>
@@ -2930,7 +2911,7 @@
         <v>4.7138115799883178E-7</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4">
       <c r="B14">
         <f t="shared" si="1"/>
         <v>2.2501177715893195</v>
@@ -2944,7 +2925,7 @@
         <v>2.2497442557269967</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4">
       <c r="B16" s="2">
         <f>SUM(B12:D14)</f>
         <v>4.4998625069898432</v>
@@ -2956,16 +2937,16 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8E82B8F-29E1-4315-852A-14C5AE3CB1A9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -2979,7 +2960,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2993,7 +2974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -3007,7 +2988,7 @@
         <v>1.9999940368885727</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -3021,7 +3002,7 @@
         <v>0.99999430923095767</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -3035,7 +3016,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -3049,7 +3030,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -3063,7 +3044,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -3077,7 +3058,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4">
       <c r="B12">
         <f>(B8-B2)^2</f>
         <v>0</v>
@@ -3091,7 +3072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4">
       <c r="B13">
         <f t="shared" ref="B13:D14" si="1">(B9-B3)^2</f>
         <v>0</v>
@@ -3105,7 +3086,7 @@
         <v>3.5558697894509646E-11</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4">
       <c r="B14">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3119,7 +3100,7 @@
         <v>3.2384852293169448E-11</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4">
       <c r="B16" s="2">
         <f>SUM(B12:D14)</f>
         <v>8.6778700869389412E-11</v>
@@ -3131,16 +3112,16 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{134DEB53-E5AB-4274-AFB9-D4C08DD6EBEC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -3154,7 +3135,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -3168,7 +3149,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -3182,7 +3163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -3196,7 +3177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -3210,7 +3191,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -3224,7 +3205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -3238,7 +3219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -3252,7 +3233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4">
       <c r="B12">
         <f>(B8-B2)^2</f>
         <v>0</v>
@@ -3266,7 +3247,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4">
       <c r="B13">
         <f t="shared" ref="B13:D14" si="1">(B9-B3)^2</f>
         <v>0</v>
@@ -3280,7 +3261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4">
       <c r="B14">
         <f t="shared" si="1"/>
         <v>2.2403791125511522E-11</v>
@@ -3294,7 +3275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4">
       <c r="B16" s="2">
         <f>SUM(B12:D14)</f>
         <v>4.6698300773274395E-11</v>
@@ -3306,16 +3287,16 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F142013-565D-4117-8E1E-C10958E38EE8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -3329,7 +3310,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -3343,7 +3324,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -3357,7 +3338,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -3371,7 +3352,7 @@
         <v>-0.50022622031849817</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -3385,7 +3366,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -3399,7 +3380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -3413,7 +3394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -3427,7 +3408,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4">
       <c r="B12">
         <f>(B8-B2)^2</f>
         <v>3.7694235587884804E-8</v>
@@ -3441,7 +3422,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4">
       <c r="B13">
         <f t="shared" ref="B13:D14" si="1">(B9-B3)^2</f>
         <v>5.2899527938223088E-7</v>
@@ -3455,7 +3436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4">
       <c r="B14">
         <f t="shared" si="1"/>
         <v>2.2508779471807325</v>
@@ -3469,7 +3450,7 @@
         <v>2.2506787121311271</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4">
       <c r="B16" s="2">
         <f>SUM(B12:D14)</f>
         <v>4.5015572260013741</v>
@@ -3481,16 +3462,16 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01013357-7328-4AD5-90E3-3258776CEF5B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -3504,7 +3485,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -3518,7 +3499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -3532,7 +3513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -3546,7 +3527,7 @@
         <v>-0.18842641396375912</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -3560,7 +3541,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -3574,7 +3555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -3588,7 +3569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -3602,7 +3583,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4">
       <c r="B12">
         <f>(B8-B2)^2</f>
         <v>0</v>
@@ -3616,7 +3597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4">
       <c r="B13">
         <f t="shared" ref="B13:D14" si="1">(B9-B3)^2</f>
         <v>0</v>
@@ -3630,7 +3611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4">
       <c r="B14">
         <f t="shared" si="1"/>
         <v>4.2805572777593568</v>
@@ -3644,13 +3625,13 @@
         <v>1.4123573414067601</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4">
       <c r="B16" s="2">
         <f>SUM(B12:D14)</f>
         <v>7.1053368112401367</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1">
       <c r="A19" s="4"/>
     </row>
   </sheetData>
@@ -3659,16 +3640,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63B97CF0-99B2-4337-A953-1577F71FE002}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -3682,7 +3663,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -3696,7 +3677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -3710,7 +3691,7 @@
         <v>2.4270519913476594E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -3724,7 +3705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -3738,7 +3719,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -3752,7 +3733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -3766,7 +3747,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -3780,7 +3761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4">
       <c r="B12">
         <f>(B8-B2)^2</f>
         <v>0</v>
@@ -3794,7 +3775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4">
       <c r="B13">
         <f t="shared" ref="B13:D14" si="1">(B9-B3)^2</f>
         <v>0.94694657218292799</v>
@@ -3808,7 +3789,7 @@
         <v>0.95204801830991725</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4">
       <c r="B14">
         <f>(B10-B4)^2</f>
         <v>4.0061068681478744</v>
@@ -3822,7 +3803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4">
       <c r="B16" s="2">
         <f>SUM(B12:D14)</f>
         <v>9.9181798458956543</v>
@@ -3834,19 +3815,19 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A76EDBDA-A255-485C-A114-9E4EBC1235F8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="15.6">
       <c r="A1" s="6" t="s">
         <v>4</v>
       </c>
@@ -3860,7 +3841,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="15.6">
       <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
@@ -3874,7 +3855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="15.6">
       <c r="A3" s="6" t="s">
         <v>6</v>
       </c>
@@ -3888,7 +3869,7 @@
         <v>2.0003228159575697</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="15.6">
       <c r="A4" s="6" t="s">
         <v>7</v>
       </c>
@@ -3902,7 +3883,7 @@
         <v>1.0000351598723789</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="14.45">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -3916,7 +3897,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="14.45">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -3930,7 +3911,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="14.45">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -3944,7 +3925,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="14.45">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -3958,7 +3939,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="14.45">
       <c r="B12">
         <f>(B8-B2)^2</f>
         <v>1.3504219167932795E-5</v>
@@ -3972,7 +3953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="14.45">
       <c r="B13">
         <f t="shared" ref="B13:D14" si="1">(B9-B3)^2</f>
         <v>0</v>
@@ -3986,7 +3967,7 @@
         <v>1.0421014246162073E-7</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="14.45">
       <c r="B14">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4000,13 +3981,13 @@
         <v>1.2362166257004066E-9</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="14.45">
       <c r="B16" s="2">
         <f>SUM(B12:D14)</f>
         <v>2.5315618223864992E-5</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" ht="14.45">
       <c r="A17" s="4">
         <v>45847</v>
       </c>
@@ -4014,7 +3995,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" ht="14.45">
       <c r="A18" s="4">
         <v>45923</v>
       </c>
@@ -4028,16 +4009,16 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{300E425B-5620-4431-B514-B1BBE2549DEE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -4051,7 +4032,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -4065,7 +4046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -4079,7 +4060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -4093,7 +4074,7 @@
         <v>1.0000175564579665</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -4107,7 +4088,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -4121,7 +4102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -4135,7 +4116,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -4149,7 +4130,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4">
       <c r="B12">
         <f>(B8-B2)^2</f>
         <v>0</v>
@@ -4163,7 +4144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4">
       <c r="B13">
         <f t="shared" ref="B13:D14" si="1">(B9-B3)^2</f>
         <v>9.4224826747076011E-10</v>
@@ -4177,7 +4158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4">
       <c r="B14">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4191,7 +4172,7 @@
         <v>3.0822921633045451E-10</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4">
       <c r="B16" s="2">
         <f>SUM(B12:D14)</f>
         <v>1.7491420541030022E-9</v>
@@ -4203,16 +4184,16 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{283F7287-090A-46B7-BA3C-27A59C785353}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -4226,7 +4207,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -4240,7 +4221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -4254,7 +4235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -4268,7 +4249,7 @@
         <v>0.9999258192369036</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -4282,7 +4263,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -4296,7 +4277,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -4310,7 +4291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -4324,7 +4305,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4">
       <c r="B12">
         <f>(B8-B2)^2</f>
         <v>0</v>
@@ -4338,7 +4319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4">
       <c r="B13">
         <f t="shared" ref="B13:D14" si="1">(B9-B3)^2</f>
         <v>0.11993824765256311</v>
@@ -4352,7 +4333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4">
       <c r="B14">
         <f t="shared" si="1"/>
         <v>1.0726439655822539</v>
@@ -4366,7 +4347,7 @@
         <v>5.50278561356402E-9</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4">
       <c r="B16" s="2">
         <f>SUM(B12:D14)</f>
         <v>1.1925822189679345</v>
@@ -4378,16 +4359,16 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4F4D67F-EBC9-4525-9562-7ED2D7D2B6E2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="15.6">
       <c r="A1" s="7" t="s">
         <v>4</v>
       </c>
@@ -4401,7 +4382,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="15.6">
       <c r="A2" s="7" t="s">
         <v>5</v>
       </c>
@@ -4415,7 +4396,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="15.6">
       <c r="A3" s="7" t="s">
         <v>6</v>
       </c>
@@ -4429,7 +4410,7 @@
         <v>-1.9999656340831122</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="15.6">
       <c r="A4" s="7" t="s">
         <v>7</v>
       </c>
@@ -4443,7 +4424,7 @@
         <v>0.99998429927942689</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="14.45">
       <c r="A7" s="8" t="s">
         <v>4</v>
       </c>
@@ -4457,7 +4438,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="14.45">
       <c r="A8" s="8" t="s">
         <v>5</v>
       </c>
@@ -4471,7 +4452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="14.45">
       <c r="A9" s="8" t="s">
         <v>6</v>
       </c>
@@ -4485,7 +4466,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="14.45">
       <c r="A10" s="8" t="s">
         <v>7</v>
       </c>
@@ -4499,7 +4480,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="14.45">
       <c r="B12">
         <f>(B8-B2)^2</f>
         <v>0</v>
@@ -4513,7 +4494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="14.45">
       <c r="B13">
         <f t="shared" ref="B13:D14" si="1">(B9-B3)^2</f>
         <v>3.2709689455611673E-11</v>
@@ -4527,7 +4508,7 @@
         <v>1.1810162435370174E-9</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="14.45">
       <c r="B14">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4541,7 +4522,7 @@
         <v>2.4651262651483444E-10</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="14.45">
       <c r="B16" s="2">
         <f>SUM(B12:D14)</f>
         <v>2.5939981710941708E-9</v>
@@ -4553,16 +4534,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0089BC1C-C5EA-49A9-99C3-DFC372691FF0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -4576,7 +4557,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -4590,7 +4571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -4604,7 +4585,7 @@
         <v>0.22305858959594416</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -4618,7 +4599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -4632,7 +4613,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -4646,7 +4627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -4660,7 +4641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -4674,7 +4655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4">
       <c r="B12">
         <f>(B8-B2)^2</f>
         <v>0</v>
@@ -4688,7 +4669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4">
       <c r="B13">
         <f t="shared" ref="B13:D14" si="1">(B9-B3)^2</f>
         <v>3.0934121484944019</v>
@@ -4702,7 +4683,7 @@
         <v>0.60363795520064356</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4">
       <c r="B14">
         <f>(B10-B4)^2</f>
         <v>0</v>
@@ -4716,7 +4697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4">
       <c r="B16" s="2">
         <f>SUM(B12:D14)</f>
         <v>4.3002266476297253</v>
@@ -4728,16 +4709,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{313B83BB-D4F2-401B-BF0B-10D69BB3D6FD}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -4751,7 +4732,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -4765,7 +4746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -4779,7 +4760,7 @@
         <v>1.0000339656771842</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -4793,7 +4774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -4807,7 +4788,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -4821,7 +4802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -4835,7 +4816,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -4849,7 +4830,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4">
       <c r="B12">
         <f>(B8-B2)^2</f>
         <v>1.0792552964615165E-8</v>
@@ -4863,7 +4844,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4">
       <c r="B13">
         <f t="shared" ref="B13:D14" si="1">(B9-B3)^2</f>
         <v>0</v>
@@ -4877,7 +4858,7 @@
         <v>1.1536672265790267E-9</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4">
       <c r="B14">
         <f>(B10-B4)^2</f>
         <v>5.0911418357998612E-9</v>
@@ -4891,7 +4872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4">
       <c r="B16" s="2">
         <f>SUM(B12:D14)</f>
         <v>3.4340534828846362E-8</v>
@@ -4903,16 +4884,16 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC3D4390-3995-460B-ABEF-C18D95517F47}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -4926,7 +4907,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -4940,7 +4921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -4954,7 +4935,7 @@
         <v>0.99928392523804233</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -4968,7 +4949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -4982,7 +4963,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -4996,7 +4977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -5010,7 +4991,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -5024,7 +5005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4">
       <c r="B12">
         <f>(B8-B2)^2</f>
         <v>0</v>
@@ -5038,7 +5019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4">
       <c r="B13">
         <f t="shared" ref="B13:D14" si="1">(B9-B3)^2</f>
         <v>0</v>
@@ -5052,7 +5033,7 @@
         <v>5.1276306471274036E-7</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4">
       <c r="B14">
         <f>(B10-B4)^2</f>
         <v>0</v>
@@ -5066,7 +5047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4">
       <c r="B16" s="2">
         <f>SUM(B12:D14)</f>
         <v>3.0404652118011022E-6</v>
@@ -5078,14 +5059,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CB9E05B-3793-41C3-B94B-40F5229BD806}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -5099,7 +5080,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -5113,7 +5094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -5127,7 +5108,7 @@
         <v>1.0001252062292589</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -5141,7 +5122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -5155,7 +5136,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -5169,7 +5150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -5183,7 +5164,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -5197,7 +5178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4">
       <c r="B12">
         <f>(B8-B2)^2</f>
         <v>2.257133838201372E-6</v>
@@ -5211,7 +5192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4">
       <c r="B13">
         <f t="shared" ref="B13:D14" si="1">(B9-B3)^2</f>
         <v>0</v>
@@ -5225,7 +5206,7 @@
         <v>1.5676599845240738E-8</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4">
       <c r="B14">
         <f>(B10-B4)^2</f>
         <v>0</v>
@@ -5239,7 +5220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4">
       <c r="B16" s="2">
         <f>SUM(B12:D14)</f>
         <v>3.6303566876897907E-6</v>
@@ -5251,16 +5232,16 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF6FF64C-47D1-4ACB-8BCD-8DB8DA890DE2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -5274,7 +5255,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -5288,7 +5269,7 @@
         <v>-0.99977725205514922</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -5302,7 +5283,7 @@
         <v>1.9996612130484597</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -5316,7 +5297,7 @@
         <v>-1.9996733189877614</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -5330,7 +5311,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -5344,7 +5325,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -5358,7 +5339,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -5372,7 +5353,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4">
       <c r="B12">
         <f>(B8-B2)^2</f>
         <v>0</v>
@@ -5386,7 +5367,7 @@
         <v>4.9616646935244487E-8</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4">
       <c r="B13">
         <f t="shared" ref="B13:D14" si="1">(B9-B3)^2</f>
         <v>0</v>
@@ -5400,7 +5381,7 @@
         <v>1.1477659853398743E-7</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4">
       <c r="B14">
         <f>(B10-B4)^2</f>
         <v>0</v>
@@ -5414,7 +5395,7 @@
         <v>1.0672048375726891E-7</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4">
       <c r="B16" s="2">
         <f>SUM(B12:D14)</f>
         <v>2.8490723934436047E-7</v>
@@ -5426,16 +5407,16 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71C51A42-0714-4274-9CCE-FD3E5D511EAB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -5449,7 +5430,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -5463,7 +5444,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -5477,7 +5458,7 @@
         <v>0.99999677456410552</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -5491,7 +5472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -5505,7 +5486,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -5519,7 +5500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -5533,7 +5514,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -5547,7 +5528,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4">
       <c r="B12">
         <f>(B8-B2)^2</f>
         <v>9.0355165274668185E-11</v>
@@ -5561,7 +5542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4">
       <c r="B13">
         <f t="shared" ref="B13:D14" si="1">(B9-B3)^2</f>
         <v>2.5667573193892489E-10</v>
@@ -5575,7 +5556,7 @@
         <v>1.040343670941783E-11</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4">
       <c r="B14">
         <f>(B10-B4)^2</f>
         <v>0</v>
@@ -5589,7 +5570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4">
       <c r="B16" s="2">
         <f>SUM(B12:D14)</f>
         <v>4.5123729600762591E-10</v>
@@ -5601,16 +5582,16 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{743B6CCE-E37A-4B9D-B598-F019BFB3039F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -5624,7 +5605,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -5638,7 +5619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -5652,7 +5633,7 @@
         <v>0.99999805152576005</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -5666,7 +5647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -5680,7 +5661,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -5694,7 +5675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -5708,7 +5689,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -5722,7 +5703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4">
       <c r="B12">
         <f>(B8-B2)^2</f>
         <v>0</v>
@@ -5736,7 +5717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4">
       <c r="B13">
         <f t="shared" ref="B13:D14" si="1">(B9-B3)^2</f>
         <v>0</v>
@@ -5750,7 +5731,7 @@
         <v>3.7965518637661828E-12</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4">
       <c r="B14">
         <f>(B10-B4)^2</f>
         <v>2.4737206257391508E-10</v>
@@ -5764,7 +5745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4">
       <c r="B16" s="2">
         <f>SUM(B12:D14)</f>
         <v>8.1226108532573268E-10</v>
@@ -5776,20 +5757,20 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="070f1269-45c1-4463-99ba-5dc4e57c7dff" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="070f1269-45c1-4463-99ba-5dc4e57c7dff" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5988,19 +5969,19 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2EE723E-1688-4D1F-8FE6-FDF46584855C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FAD4690-B959-480E-AC59-DDDE87F8E768}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="070f1269-45c1-4463-99ba-5dc4e57c7dff"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FAD4690-B959-480E-AC59-DDDE87F8E768}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2EE723E-1688-4D1F-8FE6-FDF46584855C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="070f1269-45c1-4463-99ba-5dc4e57c7dff"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>